<commit_message>
fix: implement comprehensive Oregon CGT validator improvements
- Add centralized _get_header_row() method for consistent header handling
- Fix header rows: RX_MED sheets at row 12, others at 10, PROV_ID at 8
- Add Date field validation to Cover Page (cell [15,2])
- Implement LOB code 7 restriction (only allowed in TME_ALL)
- Add PROV_ID field code validation (PRV01, [blank], PRV02)
- Implement complete data type validation for all field types
- Add case-insensitive provider/IPA matching
- Fix RX_MED_PROV cross-reference to use correct header row
- Update mock data generator to match spec.yaml structure
- Add comprehensive test coverage with 6 new test methods
- Update all Oregon documentation to reflect changes

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/cgt-validator/mock_data/oregon/test_submission_valid.xlsx
+++ b/cgt-validator/mock_data/oregon/test_submission_valid.xlsx
@@ -791,7 +791,7 @@
       <c r="B10" t="inlineStr"/>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>686579303</t>
+          <t>786579303</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -806,7 +806,7 @@
       <c r="B11" t="inlineStr"/>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>796233790</t>
+          <t>896233790</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -821,7 +821,7 @@
       <c r="B12" t="inlineStr"/>
       <c r="C12" s="1" t="inlineStr">
         <is>
-          <t>239670711</t>
+          <t>339670711</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -840,7 +840,7 @@
       </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
-          <t>110053353</t>
+          <t>210053353</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -852,14 +852,10 @@
           <t>Bend Medical Center</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>SUB IPA 1</t>
-        </is>
-      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" s="1" t="inlineStr">
         <is>
-          <t>957970516</t>
+          <t>685582861</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -874,7 +870,7 @@
       <c r="B15" t="inlineStr"/>
       <c r="C15" s="1" t="inlineStr">
         <is>
-          <t>634036506</t>
+          <t>553035110</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -889,7 +885,7 @@
       <c r="B16" t="inlineStr"/>
       <c r="C16" s="1" t="inlineStr">
         <is>
-          <t>031994523</t>
+          <t>200604502</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -908,7 +904,7 @@
       </c>
       <c r="C17" s="1" t="inlineStr">
         <is>
-          <t>249817734</t>
+          <t>642621108</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
@@ -920,14 +916,10 @@
           <t>Coastal Health Alliance</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>SUB IPA 1</t>
-        </is>
-      </c>
+      <c r="B18" t="inlineStr"/>
       <c r="C18" s="1" t="inlineStr">
         <is>
-          <t>028492780</t>
+          <t>702632297</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
@@ -946,7 +938,7 @@
       </c>
       <c r="C19" s="1" t="inlineStr">
         <is>
-          <t>768820204</t>
+          <t>797808098</t>
         </is>
       </c>
       <c r="D19" t="inlineStr"/>
@@ -1729,28 +1721,28 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>40713</v>
+        <v>32493</v>
       </c>
       <c r="D10" t="n">
-        <v>0.968</v>
+        <v>0.888</v>
       </c>
       <c r="E10" t="n">
-        <v>11800329.58</v>
+        <v>10328001.97</v>
       </c>
       <c r="F10" t="n">
-        <v>7805846.75</v>
+        <v>8819073.57</v>
       </c>
       <c r="G10" t="n">
-        <v>3805241.2</v>
+        <v>1635208.21</v>
       </c>
       <c r="H10" t="n">
-        <v>7160632.43</v>
+        <v>5867648.49</v>
       </c>
       <c r="I10" t="n">
-        <v>1009266.29</v>
+        <v>1330399.3</v>
       </c>
       <c r="J10" t="n">
-        <v>1737567</v>
+        <v>1306462.8</v>
       </c>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
@@ -1781,28 +1773,28 @@
         <v>2</v>
       </c>
       <c r="C11" t="n">
-        <v>23210</v>
+        <v>15189</v>
       </c>
       <c r="D11" t="n">
-        <v>0.862</v>
+        <v>0.886</v>
       </c>
       <c r="E11" t="n">
-        <v>9085383.08</v>
+        <v>5357142.47</v>
       </c>
       <c r="F11" t="n">
-        <v>4653353.91</v>
+        <v>2511220.78</v>
       </c>
       <c r="G11" t="n">
-        <v>1268131.55</v>
+        <v>1047985.79</v>
       </c>
       <c r="H11" t="n">
-        <v>2545478.71</v>
+        <v>2064153.78</v>
       </c>
       <c r="I11" t="n">
-        <v>1054310.33</v>
+        <v>460510.3</v>
       </c>
       <c r="J11" t="n">
-        <v>1116674.44</v>
+        <v>576204.22</v>
       </c>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
@@ -3041,11 +3033,7 @@
           <t>Bend Medical Center</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>SUB IPA 1</t>
-        </is>
-      </c>
+      <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
         <v>1</v>
       </c>
@@ -3091,11 +3079,7 @@
           <t>Bend Medical Center</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>SUB IPA 1</t>
-        </is>
-      </c>
+      <c r="D24" t="inlineStr"/>
       <c r="E24" t="n">
         <v>1</v>
       </c>
@@ -3141,11 +3125,7 @@
           <t>Bend Medical Center</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>SUB IPA 1</t>
-        </is>
-      </c>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="n">
         <v>1</v>
       </c>
@@ -3709,11 +3689,7 @@
           <t>Coastal Health Alliance</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>SUB IPA 1</t>
-        </is>
-      </c>
+      <c r="D37" t="inlineStr"/>
       <c r="E37" t="n">
         <v>1</v>
       </c>
@@ -3759,11 +3735,7 @@
           <t>Coastal Health Alliance</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>SUB IPA 1</t>
-        </is>
-      </c>
+      <c r="D38" t="inlineStr"/>
       <c r="E38" t="n">
         <v>1</v>
       </c>
@@ -3809,11 +3781,7 @@
           <t>Coastal Health Alliance</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>SUB IPA 1</t>
-        </is>
-      </c>
+      <c r="D39" t="inlineStr"/>
       <c r="E39" t="n">
         <v>1</v>
       </c>
@@ -3859,11 +3827,7 @@
           <t>Coastal Health Alliance</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>SUB IPA 1</t>
-        </is>
-      </c>
+      <c r="D40" t="inlineStr"/>
       <c r="E40" t="n">
         <v>1</v>
       </c>
@@ -5419,7 +5383,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>686579303</t>
+          <t>786579303</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -5467,7 +5431,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>686579303</t>
+          <t>786579303</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -5515,7 +5479,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>796233790</t>
+          <t>896233790</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -5563,7 +5527,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>796233790</t>
+          <t>896233790</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -5611,7 +5575,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>796233790</t>
+          <t>896233790</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -5659,7 +5623,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>239670711</t>
+          <t>339670711</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -5707,7 +5671,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>239670711</t>
+          <t>339670711</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -5755,7 +5719,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>239670711</t>
+          <t>339670711</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -5803,7 +5767,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>110053353</t>
+          <t>210053353</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -5851,7 +5815,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>110053353</t>
+          <t>210053353</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -5899,7 +5863,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>110053353</t>
+          <t>210053353</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -5947,7 +5911,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>110053353</t>
+          <t>210053353</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -5995,7 +5959,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>957970516</t>
+          <t>685582861</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -6043,7 +6007,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>957970516</t>
+          <t>685582861</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -6091,7 +6055,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>957970516</t>
+          <t>685582861</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -6139,7 +6103,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>957970516</t>
+          <t>685582861</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -6187,7 +6151,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>634036506</t>
+          <t>553035110</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -6235,7 +6199,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>634036506</t>
+          <t>553035110</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -6283,7 +6247,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>634036506</t>
+          <t>553035110</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -6331,7 +6295,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>634036506</t>
+          <t>553035110</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -6379,7 +6343,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>031994523</t>
+          <t>200604502</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -6427,7 +6391,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>031994523</t>
+          <t>200604502</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -6475,7 +6439,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>031994523</t>
+          <t>200604502</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -6523,7 +6487,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>249817734</t>
+          <t>642621108</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -6571,7 +6535,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>249817734</t>
+          <t>642621108</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -6619,7 +6583,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>249817734</t>
+          <t>642621108</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -6667,7 +6631,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>249817734</t>
+          <t>642621108</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -6715,7 +6679,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>028492780</t>
+          <t>702632297</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -6763,7 +6727,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>028492780</t>
+          <t>702632297</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -6811,7 +6775,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>028492780</t>
+          <t>702632297</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -6859,7 +6823,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>028492780</t>
+          <t>702632297</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -6907,7 +6871,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>768820204</t>
+          <t>797808098</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -6955,7 +6919,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>768820204</t>
+          <t>797808098</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -7003,7 +6967,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>768820204</t>
+          <t>797808098</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">

</xml_diff>